<commit_message>
Changed CompositeVariable to TransformVariable
</commit_message>
<xml_diff>
--- a/paper-pusher/test.xlsx
+++ b/paper-pusher/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\scrivener\scrivner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\paper-pusher\paper-pusher\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>First name</t>
   </si>
@@ -48,6 +48,18 @@
   </si>
   <si>
     <t>Demographics</t>
+  </si>
+  <si>
+    <t>Last date voted</t>
+  </si>
+  <si>
+    <t>Voting behavior</t>
+  </si>
+  <si>
+    <t>Cruz</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
 </sst>
 </file>
@@ -78,7 +90,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -110,11 +122,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -398,29 +411,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -433,8 +450,11 @@
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -447,6 +467,22 @@
       <c r="D3" s="2">
         <v>30075</v>
       </c>
+      <c r="E3" s="2">
+        <v>41223</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2">
+        <v>29125</v>
+      </c>
+      <c r="E4" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>